<commit_message>
Stable Progress Bar Prompt (You made a mess of your code.....)
</commit_message>
<xml_diff>
--- a/_output/AM/UI Results/UI Result - b1(a) VS p10(b).xlsx
+++ b/_output/AM/UI Results/UI Result - b1(a) VS p10(b).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Feature</t>
   </si>
@@ -28,6 +28,12 @@
     <t>Chi Square</t>
   </si>
   <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
     <t>Is Significant</t>
   </si>
   <si>
@@ -77,6 +83,102 @@
   </si>
   <si>
     <t>n4</t>
+  </si>
+  <si>
+    <t>[283 105] ; [ 76 142]</t>
+  </si>
+  <si>
+    <t>[206 187] ; [ 70 154]</t>
+  </si>
+  <si>
+    <t>[169 224] ; [ 51 171]</t>
+  </si>
+  <si>
+    <t>[243 145] ; [ 93 129]</t>
+  </si>
+  <si>
+    <t>[294 103] ; [123 100]</t>
+  </si>
+  <si>
+    <t>[266 132] ; [107 118]</t>
+  </si>
+  <si>
+    <t>[227 167] ; [ 85 139]</t>
+  </si>
+  <si>
+    <t>[186 203] ; [ 65 156]</t>
+  </si>
+  <si>
+    <t>[194 199] ; [ 72 150]</t>
+  </si>
+  <si>
+    <t>[177 193] ; [ 65 146]</t>
+  </si>
+  <si>
+    <t>[292 100] ; [133  92]</t>
+  </si>
+  <si>
+    <t>[238 146] ; [103 119]</t>
+  </si>
+  <si>
+    <t>[145 242] ; [ 51 168]</t>
+  </si>
+  <si>
+    <t>[286 112] ; [131  94]</t>
+  </si>
+  <si>
+    <t>[120 259] ; [ 41 176]</t>
+  </si>
+  <si>
+    <t>[302  96] ; [141  82]</t>
+  </si>
+  <si>
+    <t>[229.85478548 158.14521452] ; [129.14521452  88.85478548]</t>
+  </si>
+  <si>
+    <t>[175.79902755 217.20097245] ; [100.20097245 123.79902755]</t>
+  </si>
+  <si>
+    <t>[140.58536585 252.41463415] ; [ 79.41463415 142.58536585]</t>
+  </si>
+  <si>
+    <t>[213.71803279 174.28196721] ; [122.28196721  99.71803279]</t>
+  </si>
+  <si>
+    <t>[267.01451613 129.98548387] ; [149.98548387  73.01451613]</t>
+  </si>
+  <si>
+    <t>[238.28892456 159.71107544] ; [134.71107544  90.28892456]</t>
+  </si>
+  <si>
+    <t>[198.91262136 195.08737864] ; [113.08737864 110.91262136]</t>
+  </si>
+  <si>
+    <t>[160.06393443 228.93606557] ; [ 90.93606557 130.06393443]</t>
+  </si>
+  <si>
+    <t>[169.9804878 223.0195122] ; [ 96.0195122 125.9804878]</t>
+  </si>
+  <si>
+    <t>[154.11359725 215.88640275] ; [ 87.88640275 123.11359725]</t>
+  </si>
+  <si>
+    <t>[270.01620746 121.98379254] ; [154.98379254  70.01620746]</t>
+  </si>
+  <si>
+    <t>[216.07920792 167.92079208] ; [124.92079208  97.07920792]</t>
+  </si>
+  <si>
+    <t>[125.16831683 261.83168317] ; [ 70.83168317 148.16831683]</t>
+  </si>
+  <si>
+    <t>[266.39807384 131.60192616] ; [150.60192616  74.39807384]</t>
+  </si>
+  <si>
+    <t>[102.38087248 276.61912752] ; [ 58.61912752 158.38087248]</t>
+  </si>
+  <si>
+    <t>[283.9194847 114.0805153] ; [159.0805153  63.9194847]</t>
   </si>
 </sst>
 </file>
@@ -434,13 +536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,13 +558,19 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -473,16 +581,22 @@
       <c r="E2">
         <v>83.804354</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -493,16 +607,22 @@
       <c r="E3">
         <v>25.857904</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -513,16 +633,22 @@
       <c r="E4">
         <v>24.771037</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -533,16 +659,22 @@
       <c r="E5">
         <v>24.542312</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -553,16 +685,22 @@
       <c r="E6">
         <v>23.158372</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -573,16 +711,22 @@
       <c r="E7">
         <v>22.23599</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -593,16 +737,22 @@
       <c r="E8">
         <v>22.098744</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -613,16 +763,22 @@
       <c r="E9">
         <v>19.710047</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -633,16 +789,22 @@
       <c r="E10">
         <v>16.569184</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -653,16 +815,22 @@
       <c r="E11">
         <v>16.039256</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -673,16 +841,22 @@
       <c r="E12">
         <v>15.772553</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -693,16 +867,22 @@
       <c r="E13">
         <v>13.881804</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -713,16 +893,22 @@
       <c r="E14">
         <v>12.851151</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -733,16 +919,22 @@
       <c r="E15">
         <v>12.077937</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -753,16 +945,22 @@
       <c r="E16">
         <v>11.410206</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -773,7 +971,13 @@
       <c r="E17">
         <v>11.186256</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
     </row>

</xml_diff>